<commit_message>
Updated few modules like NGIN, IP Transit, HSS
</commit_message>
<xml_diff>
--- a/APTAutomationProject/src/com/colt/qa/datalibrary/APT_HSS.xlsx
+++ b/APTAutomationProject/src/com/colt/qa/datalibrary/APT_HSS.xlsx
@@ -377,121 +377,121 @@
     <t>9367462881</t>
   </si>
   <si>
-    <t>HSS113</t>
-  </si>
-  <si>
-    <t>hssdomain113.com</t>
-  </si>
-  <si>
-    <t>hssocn113</t>
-  </si>
-  <si>
-    <t>testreference113</t>
-  </si>
-  <si>
-    <t>hsscontact113</t>
-  </si>
-  <si>
-    <t>hss113@test.com</t>
-  </si>
-  <si>
-    <t>HSSOrder_113</t>
-  </si>
-  <si>
-    <t>HSSRFI_113</t>
-  </si>
-  <si>
-    <t>HSSService_113</t>
-  </si>
-  <si>
-    <t>HSSOrderedit_113</t>
-  </si>
-  <si>
-    <t>HSSRFIedit_113</t>
-  </si>
-  <si>
-    <t>HSS114</t>
-  </si>
-  <si>
-    <t>hssdomain114.com</t>
-  </si>
-  <si>
-    <t>hssocn114</t>
-  </si>
-  <si>
-    <t>testreference114</t>
-  </si>
-  <si>
-    <t>hsscontact114</t>
-  </si>
-  <si>
-    <t>hss114@test.com</t>
-  </si>
-  <si>
-    <t>HSSOrder_114</t>
-  </si>
-  <si>
-    <t>HSSRFI_114</t>
-  </si>
-  <si>
-    <t>HSSService_114</t>
-  </si>
-  <si>
-    <t>HSSOrderedit_114</t>
-  </si>
-  <si>
-    <t>HSSRFIedit_114</t>
-  </si>
-  <si>
-    <t>10.25.32.46</t>
-  </si>
-  <si>
-    <t>10.25.32.47</t>
-  </si>
-  <si>
-    <t>Device287</t>
-  </si>
-  <si>
-    <t>Device288</t>
-  </si>
-  <si>
-    <t>HSS118</t>
-  </si>
-  <si>
-    <t>hssdomain118.com</t>
-  </si>
-  <si>
-    <t>hssocn118</t>
-  </si>
-  <si>
-    <t>testreference118</t>
-  </si>
-  <si>
-    <t>hsscontact118</t>
-  </si>
-  <si>
-    <t>hss118@test.com</t>
-  </si>
-  <si>
-    <t>HSSOrder_118</t>
-  </si>
-  <si>
-    <t>HSSRFI_118</t>
-  </si>
-  <si>
-    <t>HSSService_118</t>
-  </si>
-  <si>
-    <t>HSSOrderedit_118</t>
-  </si>
-  <si>
-    <t>HSSRFIedit_118</t>
-  </si>
-  <si>
-    <t>Device292</t>
-  </si>
-  <si>
-    <t>10.25.34.50</t>
+    <t>HSS122</t>
+  </si>
+  <si>
+    <t>hssdomain122.com</t>
+  </si>
+  <si>
+    <t>hssocn122</t>
+  </si>
+  <si>
+    <t>testreference122</t>
+  </si>
+  <si>
+    <t>hsscontact122</t>
+  </si>
+  <si>
+    <t>hss122@test.com</t>
+  </si>
+  <si>
+    <t>HSSOrder_122</t>
+  </si>
+  <si>
+    <t>HSSRFI_122</t>
+  </si>
+  <si>
+    <t>HSSService_122</t>
+  </si>
+  <si>
+    <t>HSSOrderedit_122</t>
+  </si>
+  <si>
+    <t>HSSRFIedit_122</t>
+  </si>
+  <si>
+    <t>Device297</t>
+  </si>
+  <si>
+    <t>10.23.35.53</t>
+  </si>
+  <si>
+    <t>HSS123</t>
+  </si>
+  <si>
+    <t>hssdomain123.com</t>
+  </si>
+  <si>
+    <t>hssocn123</t>
+  </si>
+  <si>
+    <t>testreference123</t>
+  </si>
+  <si>
+    <t>hsscontact123</t>
+  </si>
+  <si>
+    <t>hss123@test.com</t>
+  </si>
+  <si>
+    <t>HSSOrder_123</t>
+  </si>
+  <si>
+    <t>HSSRFI_123</t>
+  </si>
+  <si>
+    <t>HSSService_123</t>
+  </si>
+  <si>
+    <t>HSSOrderedit_123</t>
+  </si>
+  <si>
+    <t>HSSRFIedit_123</t>
+  </si>
+  <si>
+    <t>HSS124</t>
+  </si>
+  <si>
+    <t>hssdomain124.com</t>
+  </si>
+  <si>
+    <t>hssocn124</t>
+  </si>
+  <si>
+    <t>testreference124</t>
+  </si>
+  <si>
+    <t>hsscontact124</t>
+  </si>
+  <si>
+    <t>hss124@test.com</t>
+  </si>
+  <si>
+    <t>HSSOrder_124</t>
+  </si>
+  <si>
+    <t>HSSRFI_124</t>
+  </si>
+  <si>
+    <t>HSSService_124</t>
+  </si>
+  <si>
+    <t>HSSOrderedit_124</t>
+  </si>
+  <si>
+    <t>HSSRFIedit_124</t>
+  </si>
+  <si>
+    <t>10.25.34.54</t>
+  </si>
+  <si>
+    <t>10.25.32.54</t>
+  </si>
+  <si>
+    <t>Device301</t>
+  </si>
+  <si>
+    <t>Device302</t>
   </si>
 </sst>
 </file>
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR8" sqref="AR8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -946,7 +946,9 @@
     <col min="31" max="31" width="28.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="15.140625" style="1" customWidth="1"/>
     <col min="33" max="33" width="19.28515625" style="1" customWidth="1"/>
-    <col min="34" max="43" width="9" style="1"/>
+    <col min="34" max="37" width="9" style="1"/>
+    <col min="38" max="38" width="30.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="43" width="9" style="1"/>
     <col min="44" max="44" width="19.7109375" style="1" customWidth="1"/>
     <col min="45" max="45" width="12.7109375" style="1" customWidth="1"/>
     <col min="46" max="46" width="14.28515625" style="1" customWidth="1"/>
@@ -1215,7 +1217,7 @@
     </row>
     <row r="2" spans="1:83" ht="33.75" customHeight="1">
       <c r="A2" s="17" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>97</v>
@@ -1227,31 +1229,31 @@
         <v>12</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>111</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>112</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>113</v>
@@ -1272,22 +1274,22 @@
         <v>30</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="X2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>11</v>
@@ -1317,16 +1319,16 @@
         <v>18</v>
       </c>
       <c r="AI2" s="8" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="AJ2" s="8" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="AK2" s="8" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="AL2" s="8" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="AM2" s="14" t="s">
         <v>83</v>
@@ -1356,7 +1358,7 @@
         <v>22</v>
       </c>
       <c r="AV2" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="AW2" s="11" t="s">
         <v>50</v>
@@ -1466,7 +1468,7 @@
     </row>
     <row r="3" spans="1:83" ht="33.75" customHeight="1">
       <c r="A3" s="17" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>97</v>
@@ -1478,31 +1480,31 @@
         <v>12</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>111</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>112</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="N3" s="7" t="s">
         <v>113</v>
@@ -1523,22 +1525,22 @@
         <v>30</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="X3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="Z3" s="3" t="s">
         <v>11</v>
@@ -1568,16 +1570,16 @@
         <v>18</v>
       </c>
       <c r="AI3" s="8" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="AJ3" s="8" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="AK3" s="8" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="AL3" s="8" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="AM3" s="14" t="s">
         <v>83</v>
@@ -1598,7 +1600,7 @@
         <v>12</v>
       </c>
       <c r="AS3" s="10" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="AT3" s="10" t="s">
         <v>80</v>
@@ -1607,7 +1609,7 @@
         <v>22</v>
       </c>
       <c r="AV3" s="10" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="AW3" s="11" t="s">
         <v>50</v>
@@ -1729,31 +1731,31 @@
         <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>111</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>112</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="N4" s="7" t="s">
         <v>113</v>
@@ -1774,22 +1776,22 @@
         <v>30</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="X4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="Z4" s="3" t="s">
         <v>11</v>
@@ -1819,16 +1821,16 @@
         <v>18</v>
       </c>
       <c r="AI4" s="8" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="AJ4" s="8" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="AK4" s="8" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="AL4" s="8" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="AM4" s="14" t="s">
         <v>83</v>
@@ -1849,7 +1851,7 @@
         <v>12</v>
       </c>
       <c r="AS4" s="10" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="AT4" s="10" t="s">
         <v>80</v>
@@ -1858,7 +1860,7 @@
         <v>22</v>
       </c>
       <c r="AV4" s="10" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="AW4" s="11" t="s">
         <v>50</v>

</xml_diff>